<commit_message>
S3 event notifications, event source mapping,strea,s, queues,error handling, mapper scalling - CONCEPTS
</commit_message>
<xml_diff>
--- a/Rajeshwari Progress Report.xlsx
+++ b/Rajeshwari Progress Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rapyder-my.sharepoint.com/personal/rajeshwari_jadhav_rapyder_com/Documents/Desktop/Cloud Course/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rapyder-my.sharepoint.com/personal/rajeshwari_jadhav_rapyder_com/Documents/Desktop/My Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{542EF6FC-BB1D-4C48-8EF7-1BB36BB4C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35CFC3F3-35CB-464C-8EF9-F6BE7669C31E}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{542EF6FC-BB1D-4C48-8EF7-1BB36BB4C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E7DADF8-F786-4B08-974D-910C5ACC790C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0DD7DE83-C147-4EE2-99FB-0D7E082749F9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,30 @@
   </si>
   <si>
     <t xml:space="preserve">Serverless, AWS Lambda </t>
+  </si>
+  <si>
+    <t>22-10-204</t>
+  </si>
+  <si>
+    <t>AWS Certified Developer Associate Course</t>
+  </si>
+  <si>
+    <t>Getting started, Intro, IAM &amp; CLI</t>
+  </si>
+  <si>
+    <t>EC2,ELB,VPC,S3</t>
+  </si>
+  <si>
+    <t>GIT</t>
+  </si>
+  <si>
+    <t>installing, created respository for my progress report and update my report</t>
+  </si>
+  <si>
+    <t>Syncronous Invocations, services,lambda &amp; ALB(HTTP-JSON, vice versa)</t>
+  </si>
+  <si>
+    <t>S3 event notifications, event source mapping,strea,s, queues,error handling, mapper scalling</t>
   </si>
 </sst>
 </file>
@@ -469,21 +493,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1EBD6B8-2875-401B-B0CC-BBC8EB01CF4C}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="3"/>
-    <col min="2" max="2" width="12.08984375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="5" max="5" width="82.6328125" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.90625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" customWidth="1"/>
+    <col min="5" max="5" width="62.90625" customWidth="1"/>
+    <col min="6" max="6" width="11.90625" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.45">
@@ -509,41 +531,147 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <v>45588</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.78472222222222221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B7" s="4">
         <v>45589</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F7" s="5">
         <v>0.40625</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G7" s="5">
         <v>0.4375</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C5" s="3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F8" s="5">
         <v>0.44791666666666669</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.50694444444444442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C11" s="3">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.63680555555555551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
permissions, Policies, Eventand Context Objects, Destinations,logging & Monitoring,X-Ray - CONCEPTS
</commit_message>
<xml_diff>
--- a/Rajeshwari Progress Report.xlsx
+++ b/Rajeshwari Progress Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rapyder-my.sharepoint.com/personal/rajeshwari_jadhav_rapyder_com/Documents/Desktop/My Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{542EF6FC-BB1D-4C48-8EF7-1BB36BB4C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E7DADF8-F786-4B08-974D-910C5ACC790C}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{542EF6FC-BB1D-4C48-8EF7-1BB36BB4C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE725A38-A280-4071-A2E3-B18A5583676A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0DD7DE83-C147-4EE2-99FB-0D7E082749F9}"/>
+    <workbookView xWindow="2120" yWindow="2120" windowWidth="14400" windowHeight="7270" xr2:uid="{0DD7DE83-C147-4EE2-99FB-0D7E082749F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>S3 event notifications, event source mapping,strea,s, queues,error handling, mapper scalling</t>
+  </si>
+  <si>
+    <t>permissions, Policies, Eventand Context Objects, Destinations,logging &amp; Monitoring,X-Ray</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +162,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -174,6 +178,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -493,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1EBD6B8-2875-401B-B0CC-BBC8EB01CF4C}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -674,6 +682,23 @@
         <v>0.63680555555555551</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C12" s="3">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.64236111111111116</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.69444444444444442</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
customization at Edge, CloudFront Func, Lambda@Edge, Lambda by default, VPC, lambda layers.
</commit_message>
<xml_diff>
--- a/Rajeshwari Progress Report.xlsx
+++ b/Rajeshwari Progress Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rapyder-my.sharepoint.com/personal/rajeshwari_jadhav_rapyder_com/Documents/Desktop/My Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{542EF6FC-BB1D-4C48-8EF7-1BB36BB4C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE725A38-A280-4071-A2E3-B18A5583676A}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{542EF6FC-BB1D-4C48-8EF7-1BB36BB4C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F3D665F-9D02-4C18-9F3A-B1A0BE473026}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="2120" windowWidth="14400" windowHeight="7270" xr2:uid="{0DD7DE83-C147-4EE2-99FB-0D7E082749F9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>permissions, Policies, Eventand Context Objects, Destinations,logging &amp; Monitoring,X-Ray</t>
+  </si>
+  <si>
+    <t>customization at Edge, CloudFront Func, Lambda@Edge, Lambda by default, VPC, lambda layers.</t>
   </si>
 </sst>
 </file>
@@ -501,9 +504,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1EBD6B8-2875-401B-B0CC-BBC8EB01CF4C}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -692,11 +695,28 @@
       <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>0.64236111111111116</v>
       </c>
       <c r="G12" s="6">
         <v>0.69444444444444442</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C13" s="3">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.75416666666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lambda File system Mounting, Concurrency, Ext Dependencies, Lambda & CloudFormation, Container images
</commit_message>
<xml_diff>
--- a/Rajeshwari Progress Report.xlsx
+++ b/Rajeshwari Progress Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rapyder-my.sharepoint.com/personal/rajeshwari_jadhav_rapyder_com/Documents/Desktop/My Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{542EF6FC-BB1D-4C48-8EF7-1BB36BB4C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F3D665F-9D02-4C18-9F3A-B1A0BE473026}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{542EF6FC-BB1D-4C48-8EF7-1BB36BB4C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8ADE019B-11D5-4843-9E0B-03126C45B347}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="2120" windowWidth="14400" windowHeight="7270" xr2:uid="{0DD7DE83-C147-4EE2-99FB-0D7E082749F9}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{0DD7DE83-C147-4EE2-99FB-0D7E082749F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>customization at Edge, CloudFront Func, Lambda@Edge, Lambda by default, VPC, lambda layers.</t>
+  </si>
+  <si>
+    <t>lambda File system Mounting, Concurrency, Ext Dependencies, Lambda &amp; CloudFormation, Container images</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,7 +168,6 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1EBD6B8-2875-401B-B0CC-BBC8EB01CF4C}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="F4" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -515,8 +517,8 @@
     <col min="2" max="2" width="10.08984375" customWidth="1"/>
     <col min="4" max="4" width="31.7265625" customWidth="1"/>
     <col min="5" max="5" width="62.90625" customWidth="1"/>
-    <col min="6" max="6" width="11.90625" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" customWidth="1"/>
+    <col min="6" max="6" width="11.90625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.45">
@@ -698,7 +700,7 @@
       <c r="F12" s="5">
         <v>0.64236111111111116</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>0.69444444444444442</v>
       </c>
     </row>
@@ -712,11 +714,28 @@
       <c r="E13" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>0.70833333333333337</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>0.75416666666666665</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C14" s="3">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.75694444444444442</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.78125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AWS Lambda versions, Aliases, CodeDeploy, Function URL & Security, CodeGuru Profiling, Best Practices
</commit_message>
<xml_diff>
--- a/Rajeshwari Progress Report.xlsx
+++ b/Rajeshwari Progress Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rapyder-my.sharepoint.com/personal/rajeshwari_jadhav_rapyder_com/Documents/Desktop/My Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{542EF6FC-BB1D-4C48-8EF7-1BB36BB4C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8ADE019B-11D5-4843-9E0B-03126C45B347}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{542EF6FC-BB1D-4C48-8EF7-1BB36BB4C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3486755-BF8E-460B-85B6-E37685A472A8}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{0DD7DE83-C147-4EE2-99FB-0D7E082749F9}"/>
+    <workbookView minimized="1" xWindow="2460" yWindow="2460" windowWidth="14400" windowHeight="7270" xr2:uid="{0DD7DE83-C147-4EE2-99FB-0D7E082749F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -53,12 +53,6 @@
     <t>TASK</t>
   </si>
   <si>
-    <t>start-time</t>
-  </si>
-  <si>
-    <t>end-time</t>
-  </si>
-  <si>
     <t>Learning Concetps</t>
   </si>
   <si>
@@ -102,6 +96,9 @@
   </si>
   <si>
     <t>lambda File system Mounting, Concurrency, Ext Dependencies, Lambda &amp; CloudFormation, Container images</t>
+  </si>
+  <si>
+    <t>AWS Lambda versions, Aliases, CodeDeploy, Function URL &amp; Security, CodeGuru Profiling, Best Practices</t>
   </si>
 </sst>
 </file>
@@ -151,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -168,6 +165,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -183,10 +181,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,17 +500,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1EBD6B8-2875-401B-B0CC-BBC8EB01CF4C}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="F4" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="10.08984375" customWidth="1"/>
     <col min="4" max="4" width="31.7265625" customWidth="1"/>
-    <col min="5" max="5" width="62.90625" customWidth="1"/>
+    <col min="5" max="5" width="106.453125" customWidth="1"/>
     <col min="6" max="6" width="11.90625" style="3" customWidth="1"/>
     <col min="7" max="7" width="10.7265625" style="3" customWidth="1"/>
   </cols>
@@ -537,35 +531,25 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="5">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0.75</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
@@ -578,17 +562,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.78472222222222221</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
@@ -601,17 +581,13 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.40625</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0.4375</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
@@ -620,17 +596,13 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.44791666666666669</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.45833333333333331</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
@@ -639,17 +611,13 @@
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0.50694444444444442</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
@@ -658,85 +626,84 @@
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0.50694444444444442</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0.55208333333333337</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C11" s="3">
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0.59027777777777779</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0.63680555555555551</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C12" s="3">
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0.64236111111111116</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0.69444444444444442</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C13" s="3">
         <v>7</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0.75416666666666665</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C14" s="3">
         <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0.75694444444444442</v>
-      </c>
-      <c r="G14" s="5">
-        <v>0.78125</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="6">
+        <v>45590</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>